<commit_message>
nominal nas filling repaired
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -439,12 +439,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -492,31 +492,31 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.7142877473955862</v>
+        <v>0.6783525101020478</v>
       </c>
       <c r="C4">
         <v>-1</v>
       </c>
       <c r="D4">
-        <v>0.4285754947911724</v>
+        <v>0.3567050202040956</v>
       </c>
       <c r="E4">
-        <v>0.7669778526376146</v>
+        <v>0.5754920420347929</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.5339557052752293</v>
+        <v>0.1509840840695857</v>
       </c>
       <c r="H4">
-        <v>0.562717258261934</v>
+        <v>0.7796336996336996</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.1254345165238679</v>
+        <v>0.5592673992673991</v>
       </c>
       <c r="K4">
         <v>0</v>

</xml_diff>

<commit_message>
nas for nominal simple way
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -434,17 +434,17 @@
     <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -492,31 +492,31 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.6783525101020478</v>
+        <v>0.5607188170993559</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.3567050202040956</v>
+        <v>0.1214376341987118</v>
       </c>
       <c r="E4">
-        <v>0.5754920420347929</v>
+        <v>0.7831777282599498</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.1509840840695857</v>
+        <v>0.5663554565198996</v>
       </c>
       <c r="H4">
-        <v>0.7796336996336996</v>
+        <v>0.7087799791449426</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J4">
-        <v>0.5592673992673991</v>
+        <v>0.4175599582898852</v>
       </c>
       <c r="K4">
         <v>0</v>

</xml_diff>

<commit_message>
double_columns_saving and add_sheet fuctions was moved to DS_common repo
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -434,17 +434,17 @@
     <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -492,31 +492,31 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.5607188170993559</v>
+        <v>0.7041217312852566</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>0.1214376341987118</v>
+        <v>0.4082434625705131</v>
       </c>
       <c r="E4">
-        <v>0.7831777282599498</v>
+        <v>0.5497199333020351</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.5663554565198996</v>
+        <v>0.09943986660407012</v>
       </c>
       <c r="H4">
-        <v>0.7087799791449426</v>
+        <v>0.7741065466434253</v>
       </c>
       <c r="I4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.4175599582898852</v>
+        <v>0.5482130932868505</v>
       </c>
       <c r="K4">
         <v>0</v>

</xml_diff>

<commit_message>
old commit bugs fixed
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -434,12 +434,12 @@
     <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -492,31 +492,31 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.7041217312852566</v>
+        <v>0.523252976771423</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.04650595354284603</v>
+      </c>
+      <c r="E4">
+        <v>0.7361990430222111</v>
+      </c>
+      <c r="F4">
         <v>-1</v>
       </c>
-      <c r="D4">
-        <v>0.4082434625705131</v>
-      </c>
-      <c r="E4">
-        <v>0.5497199333020351</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
       <c r="G4">
-        <v>0.09943986660407012</v>
+        <v>0.4723980860444221</v>
       </c>
       <c r="H4">
-        <v>0.7741065466434253</v>
+        <v>0.7699568058175457</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.5482130932868505</v>
+        <v>0.5399136116350913</v>
       </c>
       <c r="K4">
         <v>0</v>

</xml_diff>

<commit_message>
testing notebook look great
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Hello World</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>AUC</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KS_p_val</t>
   </si>
   <si>
     <t>rel_type</t>
@@ -409,13 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,32 +436,44 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:18">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -467,70 +485,106 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="O3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.523252976771423</v>
+        <v>0.6672579313598301</v>
       </c>
       <c r="C4">
+        <v>0.2567283877815781</v>
+      </c>
+      <c r="D4">
+        <v>8.269514585912733E-13</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>0.3345158627196603</v>
+      </c>
+      <c r="G4">
+        <v>0.5114372523010396</v>
+      </c>
+      <c r="H4">
+        <v>0.05426762237393468</v>
+      </c>
+      <c r="I4">
+        <v>0.4453581064200309</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>0.04650595354284603</v>
-      </c>
-      <c r="E4">
-        <v>0.7361990430222111</v>
-      </c>
-      <c r="F4">
-        <v>-1</v>
-      </c>
-      <c r="G4">
-        <v>0.4723980860444221</v>
-      </c>
-      <c r="H4">
-        <v>0.7699568058175457</v>
-      </c>
-      <c r="I4">
+      <c r="K4">
+        <v>0.02287450460207929</v>
+      </c>
+      <c r="L4">
+        <v>0.7777352260348585</v>
+      </c>
+      <c r="M4">
+        <v>0.4580610021786492</v>
+      </c>
+      <c r="N4">
+        <v>3.679283183917694E-23</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>0.5399136116350913</v>
-      </c>
-      <c r="K4">
+      <c r="P4">
+        <v>0.5554704520697169</v>
+      </c>
+      <c r="Q4">
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
emptys by Y cats added
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>Hello World</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t>GINI</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Empty% in level</t>
+  </si>
+  <si>
+    <t>Empty% in all Empty</t>
   </si>
   <si>
     <t>numeric_variable</t>
@@ -415,13 +424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +454,17 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:30">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>1</v>
@@ -456,30 +474,39 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="2">
-        <v>2</v>
-      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="2">
+        <v>2</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:30">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -497,118 +524,172 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="AA3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:30">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>0.5257397747769708</v>
+        <v>0.5151886931344163</v>
       </c>
       <c r="C4">
-        <v>0.06963876566080041</v>
+        <v>0.06024766485089394</v>
       </c>
       <c r="D4">
-        <v>0.175452817478935</v>
+        <v>0.3231387497223792</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.05147954955394152</v>
+        <v>0.03037738626883257</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>574</v>
       </c>
       <c r="H4">
-        <v>0.6904617371027731</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.2939141662330655</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>2.041412080663211E-16</v>
+        <v>0</v>
       </c>
       <c r="K4">
+        <v>0.6916966180981214</v>
+      </c>
+      <c r="L4">
+        <v>0.2957859205901799</v>
+      </c>
+      <c r="M4">
+        <v>4.412458392712792E-16</v>
+      </c>
+      <c r="N4">
         <v>-1</v>
       </c>
-      <c r="L4">
-        <v>0.3809234742055463</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0.769316264278297</v>
-      </c>
       <c r="O4">
-        <v>0.4225726895119418</v>
+        <v>0.3833932361962429</v>
       </c>
       <c r="P4">
-        <v>1.963681450090185E-20</v>
+        <v>279</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0.777910695344961</v>
+      </c>
+      <c r="U4">
+        <v>0.4515316091266518</v>
+      </c>
+      <c r="V4">
+        <v>8.705849996169642E-24</v>
+      </c>
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="R4">
-        <v>0.538632528556594</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
+      <c r="X4">
+        <v>0.5558213906899221</v>
+      </c>
+      <c r="Y4">
+        <v>147</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="T2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
empty in nominal mistake is corrected
</commit_message>
<xml_diff>
--- a/test_result/double_header_saver.xlsx
+++ b/test_result/double_header_saver.xlsx
@@ -467,7 +467,7 @@
     <row r="2" spans="1:30">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -478,7 +478,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -597,49 +597,49 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.5151886931344163</v>
+        <v>0.7052419430788646</v>
       </c>
       <c r="C4">
-        <v>0.06024766485089394</v>
+        <v>0.2992315081652258</v>
       </c>
       <c r="D4">
-        <v>0.3231387497223792</v>
+        <v>2.49770031077616E-17</v>
       </c>
       <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>0.4104838861577291</v>
+      </c>
+      <c r="G4">
+        <v>306</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.5644922286617492</v>
+      </c>
+      <c r="L4">
+        <v>0.1144296628029505</v>
+      </c>
+      <c r="M4">
+        <v>0.003151239620582965</v>
+      </c>
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0.03037738626883257</v>
-      </c>
-      <c r="G4">
-        <v>574</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0.6916966180981214</v>
-      </c>
-      <c r="L4">
-        <v>0.2957859205901799</v>
-      </c>
-      <c r="M4">
-        <v>4.412458392712792E-16</v>
-      </c>
-      <c r="N4">
-        <v>-1</v>
-      </c>
       <c r="O4">
-        <v>0.3833932361962429</v>
+        <v>0.1289844573234984</v>
       </c>
       <c r="P4">
-        <v>279</v>
+        <v>584</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -651,22 +651,22 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0.777910695344961</v>
+        <v>0.7851685393258426</v>
       </c>
       <c r="U4">
-        <v>0.4515316091266518</v>
+        <v>0.4502553626149131</v>
       </c>
       <c r="V4">
-        <v>8.705849996169642E-24</v>
+        <v>1.186355338027967E-18</v>
       </c>
       <c r="W4">
         <v>1</v>
       </c>
       <c r="X4">
-        <v>0.5558213906899221</v>
+        <v>0.5703370786516853</v>
       </c>
       <c r="Y4">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="Z4">
         <v>0</v>

</xml_diff>